<commit_message>
Tabelas com medias Testes
</commit_message>
<xml_diff>
--- a/NovosTestes.xlsx
+++ b/NovosTestes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amserra/Documents/GitHub/Projeto-IAA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Documents\GitHub\Projeto-IAA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336FF983-DC38-534B-971A-66885081286B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F79CB0-89FC-48F3-9FDB-F4FCAC62F279}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="4" xr2:uid="{9266D7C5-1358-47E0-9573-E3ABA5B9D78F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{9266D7C5-1358-47E0-9573-E3ABA5B9D78F}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapa1a" sheetId="7" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="120">
   <si>
     <t>Mapa 1a</t>
   </si>
@@ -378,6 +378,30 @@
   <si>
     <t xml:space="preserve">Tempo mínimo(sem tocar em nada): </t>
   </si>
+  <si>
+    <t>Tempo Médio (BlockDetector = Linear):</t>
+  </si>
+  <si>
+    <t>Tempo Médio (BlockDetector = Gaussiana):</t>
+  </si>
+  <si>
+    <t>Tempo Médio (BlockDetector = Neg Logaritmico):</t>
+  </si>
+  <si>
+    <t>Tempo Médio (ResourceDetector = Linear):</t>
+  </si>
+  <si>
+    <t>Tempo Médio (ResourceDetector = Gaussiana):</t>
+  </si>
+  <si>
+    <t>Tempo Médio (ResourceDetector = Neg Logaritmico):</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tempo Médio Total = </t>
+  </si>
 </sst>
 </file>
 
@@ -534,7 +558,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -633,6 +657,10 @@
     </xf>
     <xf numFmtId="20" fontId="2" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -956,32 +984,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48915A02-5BCF-40D7-ADBB-E4C89EB67C48}">
   <dimension ref="A1:Z284"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:F32"/>
+    <sheetView topLeftCell="V19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D42" sqref="A35:D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.6640625" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
     <col min="13" max="13" width="13.33203125" customWidth="1"/>
-    <col min="14" max="14" width="13.1640625" customWidth="1"/>
-    <col min="15" max="15" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="15.5" customWidth="1"/>
-    <col min="18" max="18" width="3.1640625" customWidth="1"/>
+    <col min="14" max="14" width="13.109375" customWidth="1"/>
+    <col min="15" max="15" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="15.44140625" customWidth="1"/>
+    <col min="18" max="18" width="3.109375" customWidth="1"/>
     <col min="19" max="19" width="19" customWidth="1"/>
-    <col min="20" max="20" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="39.109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="39.6640625" customWidth="1"/>
     <col min="22" max="22" width="19" customWidth="1"/>
     <col min="23" max="23" width="11" customWidth="1"/>
-    <col min="24" max="24" width="50.5" customWidth="1"/>
+    <col min="24" max="24" width="50.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -2192,7 +2220,7 @@
       </c>
       <c r="X23" s="22"/>
     </row>
-    <row r="24" spans="1:24" ht="80">
+    <row r="24" spans="1:24" ht="72">
       <c r="A24" s="11" t="s">
         <v>4</v>
       </c>
@@ -2262,7 +2290,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:24" ht="96">
+    <row r="25" spans="1:24" ht="86.4">
       <c r="A25" s="11" t="s">
         <v>4</v>
       </c>
@@ -2470,7 +2498,7 @@
       <c r="V29" s="3"/>
       <c r="W29" s="3"/>
     </row>
-    <row r="30" spans="1:24" ht="26">
+    <row r="30" spans="1:24" ht="25.8">
       <c r="A30" s="40" t="s">
         <v>110</v>
       </c>
@@ -2517,7 +2545,7 @@
       <c r="U31" s="3"/>
       <c r="V31" s="3"/>
     </row>
-    <row r="32" spans="1:24" ht="26">
+    <row r="32" spans="1:24" ht="25.8">
       <c r="A32" s="40" t="s">
         <v>111</v>
       </c>
@@ -2564,7 +2592,7 @@
       <c r="U33" s="3"/>
       <c r="V33" s="3"/>
     </row>
-    <row r="34" spans="1:22" ht="26">
+    <row r="34" spans="1:22" ht="24.6">
       <c r="A34" s="40"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -2587,12 +2615,17 @@
       <c r="V34" s="3"/>
     </row>
     <row r="35" spans="1:22">
-      <c r="A35" s="2"/>
+      <c r="A35" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
+      <c r="E35" s="3">
+        <f>(W8+W9+W11)/3</f>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="F35" s="45"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="J35" s="2"/>
@@ -2609,12 +2642,17 @@
       <c r="V35" s="3"/>
     </row>
     <row r="36" spans="1:22">
-      <c r="A36" s="2"/>
+      <c r="A36" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
+      <c r="E36" s="3">
+        <f xml:space="preserve"> (W14 + W19 + W23) / 3</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="F36" s="45"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="J36" s="2"/>
@@ -2631,12 +2669,16 @@
       <c r="V36" s="3"/>
     </row>
     <row r="37" spans="1:22">
-      <c r="A37" s="2"/>
+      <c r="A37" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
+      <c r="E37" s="3">
+        <f>(W24 + W25 + W26) /3</f>
+        <v>8</v>
+      </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="J37" s="2"/>
@@ -2653,12 +2695,17 @@
       <c r="V37" s="3"/>
     </row>
     <row r="38" spans="1:22">
-      <c r="A38" s="2"/>
+      <c r="A38" s="2" t="s">
+        <v>115</v>
+      </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
+      <c r="E38" s="3">
+        <f xml:space="preserve"> (W8 + W14 + W23 )/3</f>
+        <v>10</v>
+      </c>
+      <c r="F38" s="45"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="J38" s="2"/>
@@ -2675,12 +2722,17 @@
       <c r="V38" s="3"/>
     </row>
     <row r="39" spans="1:22">
-      <c r="A39" s="2"/>
+      <c r="A39" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
+      <c r="E39" s="3">
+        <f xml:space="preserve"> (W9 + W19 + W25) /3</f>
+        <v>8</v>
+      </c>
+      <c r="F39" s="45"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="J39" s="2"/>
@@ -2697,12 +2749,17 @@
       <c r="V39" s="3"/>
     </row>
     <row r="40" spans="1:22">
-      <c r="A40" s="2"/>
+      <c r="A40" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
+      <c r="E40" s="3">
+        <f>(W11+W23+W26)/3</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="F40" s="45"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="J40" s="2"/>
@@ -2724,7 +2781,6 @@
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="J41" s="2"/>
@@ -2741,12 +2797,17 @@
       <c r="V41" s="3"/>
     </row>
     <row r="42" spans="1:22">
-      <c r="A42" s="2"/>
+      <c r="A42" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
+      <c r="E42" s="3">
+        <f xml:space="preserve"> (W8+W9+W11+W14+W19+W23+W24+W25+W26)/9</f>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="F42" s="45"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="J42" s="2"/>
@@ -7685,27 +7746,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE23F7D2-EBE1-4007-8C0F-8BEE0171E58C}">
   <dimension ref="A1:AD291"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="W34" sqref="W34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" customWidth="1"/>
     <col min="6" max="9" width="15.6640625" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="11" max="11" width="15.5" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" customWidth="1"/>
     <col min="13" max="13" width="13.33203125" customWidth="1"/>
-    <col min="14" max="14" width="13.1640625" customWidth="1"/>
-    <col min="15" max="17" width="13.83203125" customWidth="1"/>
-    <col min="18" max="18" width="4.1640625" customWidth="1"/>
+    <col min="14" max="14" width="13.109375" customWidth="1"/>
+    <col min="15" max="17" width="13.77734375" customWidth="1"/>
+    <col min="18" max="18" width="4.109375" customWidth="1"/>
     <col min="19" max="19" width="17.33203125" customWidth="1"/>
     <col min="20" max="20" width="37.6640625" customWidth="1"/>
-    <col min="21" max="21" width="37.83203125" customWidth="1"/>
-    <col min="22" max="22" width="19.83203125" customWidth="1"/>
+    <col min="21" max="21" width="37.77734375" customWidth="1"/>
+    <col min="22" max="22" width="19.77734375" customWidth="1"/>
     <col min="23" max="23" width="9.6640625" customWidth="1"/>
     <col min="24" max="24" width="159.33203125" customWidth="1"/>
   </cols>
@@ -8507,9 +8568,6 @@
       <c r="W16" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="X16" s="22" t="s">
-        <v>56</v>
-      </c>
       <c r="Y16" s="22"/>
       <c r="Z16" s="22"/>
       <c r="AA16" s="22"/>
@@ -8517,7 +8575,7 @@
       <c r="AC16" s="22"/>
       <c r="AD16" s="22"/>
     </row>
-    <row r="17" spans="1:24" ht="64">
+    <row r="17" spans="1:24">
       <c r="A17" s="10"/>
       <c r="B17" s="3">
         <v>0.5</v>
@@ -8579,9 +8637,6 @@
       <c r="W17" s="17">
         <v>19</v>
       </c>
-      <c r="X17" s="23" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="18" spans="1:24">
       <c r="A18" s="10"/>
@@ -8645,9 +8700,6 @@
       <c r="W18" s="17">
         <v>15</v>
       </c>
-      <c r="X18" s="22" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="19" spans="1:24">
       <c r="A19" s="10"/>
@@ -9491,9 +9543,11 @@
       <c r="W31" s="3">
         <v>11</v>
       </c>
-      <c r="X31" s="22"/>
-    </row>
-    <row r="32" spans="1:24">
+      <c r="X31" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" ht="57.6">
       <c r="A32" s="11" t="s">
         <v>4</v>
       </c>
@@ -9559,7 +9613,9 @@
       <c r="W32" s="3">
         <v>16</v>
       </c>
-      <c r="X32" s="22"/>
+      <c r="X32" s="23" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="33" spans="1:24">
       <c r="A33" s="11" t="s">
@@ -9627,7 +9683,9 @@
       <c r="W33" s="3">
         <v>11</v>
       </c>
-      <c r="X33" s="22"/>
+      <c r="X33" s="22" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="34" spans="1:24">
       <c r="A34" s="2"/>
@@ -9685,7 +9743,7 @@
       <c r="N36" s="3"/>
       <c r="X36" s="22"/>
     </row>
-    <row r="37" spans="1:24" ht="26">
+    <row r="37" spans="1:24" ht="25.8">
       <c r="A37" s="40" t="s">
         <v>110</v>
       </c>
@@ -9720,7 +9778,7 @@
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
     </row>
-    <row r="39" spans="1:24" ht="26">
+    <row r="39" spans="1:24" ht="25.8">
       <c r="A39" s="40" t="s">
         <v>111</v>
       </c>
@@ -9756,11 +9814,16 @@
       <c r="N40" s="3"/>
     </row>
     <row r="41" spans="1:24">
-      <c r="A41" s="2"/>
+      <c r="A41" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
+      <c r="E41" s="3">
+        <f>(W9 + W10 + W12)/3</f>
+        <v>11</v>
+      </c>
       <c r="F41" s="16"/>
       <c r="G41" s="16"/>
       <c r="H41" s="16"/>
@@ -9772,11 +9835,16 @@
       <c r="N41" s="3"/>
     </row>
     <row r="42" spans="1:24">
-      <c r="A42" s="2"/>
+      <c r="A42" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
+      <c r="E42" s="3">
+        <f xml:space="preserve"> (W21 + W26 + W30)/3</f>
+        <v>16.666666666666668</v>
+      </c>
       <c r="F42" s="16"/>
       <c r="G42" s="16"/>
       <c r="H42" s="16"/>
@@ -9788,11 +9856,16 @@
       <c r="N42" s="3"/>
     </row>
     <row r="43" spans="1:24">
-      <c r="A43" s="2"/>
+      <c r="A43" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
+      <c r="E43" s="3">
+        <f>W33</f>
+        <v>11</v>
+      </c>
       <c r="J43" s="2"/>
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
@@ -9800,11 +9873,16 @@
       <c r="N43" s="3"/>
     </row>
     <row r="44" spans="1:24">
-      <c r="A44" s="2"/>
+      <c r="A44" s="2" t="s">
+        <v>115</v>
+      </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
+      <c r="E44" s="3">
+        <f>(W9 + W21)/2</f>
+        <v>13.5</v>
+      </c>
       <c r="J44" s="2"/>
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
@@ -9812,11 +9890,16 @@
       <c r="N44" s="3"/>
     </row>
     <row r="45" spans="1:24">
-      <c r="A45" s="2"/>
+      <c r="A45" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
+      <c r="E45" s="3">
+        <f>(W10+W26)/2</f>
+        <v>14</v>
+      </c>
       <c r="J45" s="2"/>
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
@@ -9824,11 +9907,16 @@
       <c r="N45" s="3"/>
     </row>
     <row r="46" spans="1:24">
-      <c r="A46" s="2"/>
+      <c r="A46" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
+      <c r="E46" s="3">
+        <f>(W12 + W30 + W33)/3</f>
+        <v>13</v>
+      </c>
       <c r="J46" s="2"/>
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
@@ -9848,11 +9936,16 @@
       <c r="N47" s="3"/>
     </row>
     <row r="48" spans="1:24">
-      <c r="A48" s="2"/>
+      <c r="A48" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
+      <c r="E48" s="3">
+        <f xml:space="preserve"> (W9+W10+W12+W21+W26+W30+W33)/7</f>
+        <v>13.428571428571429</v>
+      </c>
       <c r="J48" s="2"/>
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
@@ -12664,28 +12757,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A2B7CF6-F505-4CB8-BD1F-C01EE61B21AB}">
   <dimension ref="A1:U274"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" customWidth="1"/>
     <col min="6" max="8" width="15.6640625" customWidth="1"/>
-    <col min="9" max="9" width="3.83203125" customWidth="1"/>
-    <col min="10" max="10" width="17.83203125" customWidth="1"/>
+    <col min="9" max="9" width="3.77734375" customWidth="1"/>
+    <col min="10" max="10" width="17.77734375" customWidth="1"/>
     <col min="11" max="11" width="42" customWidth="1"/>
-    <col min="12" max="12" width="20.1640625" customWidth="1"/>
-    <col min="13" max="13" width="13.1640625" customWidth="1"/>
-    <col min="14" max="14" width="158.5" customWidth="1"/>
-    <col min="15" max="15" width="4.1640625" customWidth="1"/>
+    <col min="12" max="12" width="20.109375" customWidth="1"/>
+    <col min="13" max="13" width="13.109375" customWidth="1"/>
+    <col min="14" max="14" width="158.44140625" customWidth="1"/>
+    <col min="15" max="15" width="4.109375" customWidth="1"/>
     <col min="16" max="16" width="17.33203125" customWidth="1"/>
     <col min="17" max="17" width="37.6640625" customWidth="1"/>
-    <col min="18" max="18" width="37.83203125" customWidth="1"/>
-    <col min="19" max="19" width="19.83203125" customWidth="1"/>
+    <col min="18" max="18" width="37.77734375" customWidth="1"/>
+    <col min="19" max="19" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -13079,7 +13172,7 @@
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:13" ht="26">
+    <row r="21" spans="1:13" ht="25.8">
       <c r="A21" s="40" t="s">
         <v>110</v>
       </c>
@@ -13111,7 +13204,7 @@
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13" ht="26">
+    <row r="23" spans="1:13" ht="25.8">
       <c r="A23" s="40" t="s">
         <v>111</v>
       </c>
@@ -16035,27 +16128,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE4904D-A21F-43E7-AB1D-D8515408F75D}">
   <dimension ref="A1:X284"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="X24" sqref="X24:X26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" customWidth="1"/>
     <col min="6" max="9" width="15.6640625" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="11" max="11" width="15.5" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" customWidth="1"/>
     <col min="13" max="13" width="13.33203125" customWidth="1"/>
-    <col min="14" max="14" width="13.1640625" customWidth="1"/>
-    <col min="15" max="17" width="13.83203125" customWidth="1"/>
-    <col min="18" max="18" width="4.1640625" customWidth="1"/>
+    <col min="14" max="14" width="13.109375" customWidth="1"/>
+    <col min="15" max="17" width="13.77734375" customWidth="1"/>
+    <col min="18" max="18" width="4.109375" customWidth="1"/>
     <col min="19" max="19" width="17.33203125" customWidth="1"/>
     <col min="20" max="20" width="37.6640625" customWidth="1"/>
-    <col min="21" max="21" width="37.83203125" customWidth="1"/>
-    <col min="22" max="22" width="19.83203125" customWidth="1"/>
+    <col min="21" max="21" width="37.77734375" customWidth="1"/>
+    <col min="22" max="22" width="19.77734375" customWidth="1"/>
     <col min="24" max="24" width="78" customWidth="1"/>
   </cols>
   <sheetData>
@@ -16811,9 +16904,6 @@
       <c r="W16" s="3">
         <v>32</v>
       </c>
-      <c r="X16" s="22" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="17" spans="1:24">
       <c r="A17" s="10" t="s">
@@ -16880,9 +16970,6 @@
       </c>
       <c r="W17" s="3">
         <v>34</v>
-      </c>
-      <c r="X17" s="22" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:24">
@@ -16947,9 +17034,6 @@
       <c r="W18" s="3">
         <v>24</v>
       </c>
-      <c r="X18" s="22" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="19" spans="1:24">
       <c r="A19" s="10"/>
@@ -17341,7 +17425,9 @@
       <c r="W24" s="3">
         <v>31</v>
       </c>
-      <c r="X24" s="22"/>
+      <c r="X24" s="22" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="25" spans="1:24">
       <c r="A25" s="11" t="s">
@@ -17409,7 +17495,9 @@
       <c r="W25" s="3">
         <v>41</v>
       </c>
-      <c r="X25" s="22"/>
+      <c r="X25" s="22" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="26" spans="1:24">
       <c r="A26" s="11" t="s">
@@ -17477,7 +17565,9 @@
       <c r="W26" s="3">
         <v>35</v>
       </c>
-      <c r="X26" s="22"/>
+      <c r="X26" s="22" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="27" spans="1:24">
       <c r="A27" s="2"/>
@@ -17540,7 +17630,7 @@
       <c r="V29" s="3"/>
       <c r="W29" s="3"/>
     </row>
-    <row r="30" spans="1:24" ht="26">
+    <row r="30" spans="1:24" ht="25.8">
       <c r="A30" s="42" t="s">
         <v>110</v>
       </c>
@@ -17578,7 +17668,7 @@
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
     </row>
-    <row r="32" spans="1:24" ht="26">
+    <row r="32" spans="1:24" ht="25.8">
       <c r="A32" s="42" t="s">
         <v>111</v>
       </c>
@@ -17615,11 +17705,16 @@
       <c r="N33" s="3"/>
     </row>
     <row r="34" spans="1:14">
-      <c r="A34" s="2"/>
+      <c r="A34" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
+      <c r="E34" s="3">
+        <f>(W8+W10+W12)/3</f>
+        <v>35</v>
+      </c>
       <c r="F34" s="16"/>
       <c r="G34" s="16"/>
       <c r="H34" s="16"/>
@@ -17631,11 +17726,16 @@
       <c r="N34" s="3"/>
     </row>
     <row r="35" spans="1:14">
-      <c r="A35" s="2"/>
+      <c r="A35" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
+      <c r="E35" s="3">
+        <f>(W16+W17+W23)/3</f>
+        <v>30.333333333333332</v>
+      </c>
       <c r="F35" s="16"/>
       <c r="G35" s="16"/>
       <c r="H35" s="16"/>
@@ -17647,11 +17747,16 @@
       <c r="N35" s="3"/>
     </row>
     <row r="36" spans="1:14">
-      <c r="A36" s="2"/>
+      <c r="A36" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
+      <c r="E36" s="3">
+        <f>(W24+W25+W26)/3</f>
+        <v>35.666666666666664</v>
+      </c>
       <c r="J36" s="2"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
@@ -17659,11 +17764,16 @@
       <c r="N36" s="3"/>
     </row>
     <row r="37" spans="1:14">
-      <c r="A37" s="2"/>
+      <c r="A37" s="2" t="s">
+        <v>115</v>
+      </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
+      <c r="E37" s="3">
+        <f>(W8+W16+W24)/3</f>
+        <v>34</v>
+      </c>
       <c r="J37" s="2"/>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
@@ -17671,11 +17781,16 @@
       <c r="N37" s="3"/>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="2"/>
+      <c r="A38" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
+      <c r="E38" s="3">
+        <f>(W10+W17+W25)/3</f>
+        <v>36</v>
+      </c>
       <c r="J38" s="2"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
@@ -17683,11 +17798,16 @@
       <c r="N38" s="3"/>
     </row>
     <row r="39" spans="1:14">
-      <c r="A39" s="2"/>
+      <c r="A39" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
+      <c r="E39" s="3">
+        <f>(W12+W23+W26)/3</f>
+        <v>31</v>
+      </c>
       <c r="J39" s="2"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
@@ -17707,11 +17827,16 @@
       <c r="N40" s="3"/>
     </row>
     <row r="41" spans="1:14">
-      <c r="A41" s="2"/>
+      <c r="A41" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
+      <c r="E41" s="3">
+        <f>(W8+W10+W12+W16+W17+W23+W24+W25+W26)/9</f>
+        <v>33.666666666666664</v>
+      </c>
       <c r="J41" s="2"/>
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
@@ -20523,26 +20648,26 @@
   <dimension ref="A1:AC278"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" customWidth="1"/>
     <col min="6" max="9" width="15.6640625" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="11" max="11" width="15.5" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" customWidth="1"/>
     <col min="13" max="13" width="13.33203125" customWidth="1"/>
-    <col min="14" max="14" width="13.1640625" customWidth="1"/>
-    <col min="15" max="17" width="13.83203125" customWidth="1"/>
-    <col min="18" max="18" width="4.1640625" customWidth="1"/>
+    <col min="14" max="14" width="13.109375" customWidth="1"/>
+    <col min="15" max="17" width="13.77734375" customWidth="1"/>
+    <col min="18" max="18" width="4.109375" customWidth="1"/>
     <col min="19" max="19" width="17.33203125" customWidth="1"/>
     <col min="20" max="20" width="37.6640625" customWidth="1"/>
-    <col min="21" max="21" width="37.83203125" customWidth="1"/>
-    <col min="22" max="22" width="19.83203125" customWidth="1"/>
+    <col min="21" max="21" width="37.77734375" customWidth="1"/>
+    <col min="22" max="22" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
@@ -21780,7 +21905,7 @@
       <c r="AB26" s="3"/>
       <c r="AC26" s="3"/>
     </row>
-    <row r="27" spans="1:29" ht="26">
+    <row r="27" spans="1:29" ht="25.8">
       <c r="A27" s="42" t="s">
         <v>110</v>
       </c>
@@ -21819,7 +21944,7 @@
       <c r="N28" s="3"/>
       <c r="X28" s="22"/>
     </row>
-    <row r="29" spans="1:29" ht="26">
+    <row r="29" spans="1:29" ht="25.8">
       <c r="A29" s="42" t="s">
         <v>111</v>
       </c>
@@ -21852,11 +21977,16 @@
       <c r="N30" s="3"/>
     </row>
     <row r="31" spans="1:29">
-      <c r="A31" s="2"/>
+      <c r="A31" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
+      <c r="E31" s="45">
+        <f xml:space="preserve"> (W8 + W10 + W12)/3</f>
+        <v>3.9120370370370375E-2</v>
+      </c>
       <c r="J31" s="2"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
@@ -21864,11 +21994,16 @@
       <c r="N31" s="3"/>
     </row>
     <row r="32" spans="1:29">
-      <c r="A32" s="2"/>
+      <c r="A32" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
+      <c r="E32" s="45">
+        <f>(W14 + W15 + W17) / 3</f>
+        <v>3.2638888888888891E-2</v>
+      </c>
       <c r="J32" s="2"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
@@ -21876,11 +22011,15 @@
       <c r="N32" s="3"/>
     </row>
     <row r="33" spans="1:14">
-      <c r="A33" s="2"/>
+      <c r="A33" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
+      <c r="E33" s="46" t="s">
+        <v>118</v>
+      </c>
       <c r="J33" s="2"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
@@ -21888,11 +22027,16 @@
       <c r="N33" s="3"/>
     </row>
     <row r="34" spans="1:14">
-      <c r="A34" s="2"/>
+      <c r="A34" s="2" t="s">
+        <v>115</v>
+      </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
+      <c r="E34" s="45">
+        <f>(W8 + W14)/2</f>
+        <v>4.3055555555555555E-2</v>
+      </c>
       <c r="J34" s="2"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
@@ -21900,11 +22044,16 @@
       <c r="N34" s="3"/>
     </row>
     <row r="35" spans="1:14">
-      <c r="A35" s="2"/>
+      <c r="A35" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
+      <c r="E35" s="45">
+        <f>(W10+W15)/2</f>
+        <v>3.229166666666667E-2</v>
+      </c>
       <c r="J35" s="2"/>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
@@ -21912,11 +22061,16 @@
       <c r="N35" s="3"/>
     </row>
     <row r="36" spans="1:14">
-      <c r="A36" s="2"/>
+      <c r="A36" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
+      <c r="E36" s="45">
+        <f>(W12+W17)/2</f>
+        <v>3.229166666666667E-2</v>
+      </c>
       <c r="J36" s="2"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
@@ -21928,7 +22082,6 @@
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
       <c r="J37" s="2"/>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
@@ -21936,11 +22089,16 @@
       <c r="N37" s="3"/>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="2"/>
+      <c r="A38" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
+      <c r="E38" s="45">
+        <f>(W8 + W10 + W12  + W14 + W15 + W17)/6</f>
+        <v>3.5879629629629629E-2</v>
+      </c>
       <c r="J38" s="2"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>

</xml_diff>